<commit_message>
Added Top-1 and Top-5 accuracy for Image 1 - 18
</commit_message>
<xml_diff>
--- a/model_comparison/model_comparison.xlsx
+++ b/model_comparison/model_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444BF76E-AE00-4294-830A-6D748C8A4BCE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0328450A-1F5D-453F-8F3F-AC38DAF537E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="7" xr2:uid="{5CEAE545-A299-4C48-92E4-DD670355EE21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{5CEAE545-A299-4C48-92E4-DD670355EE21}"/>
   </bookViews>
   <sheets>
     <sheet name="VGG 16" sheetId="1" r:id="rId1"/>
@@ -1949,7 +1949,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1961,6 +1961,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1983,17 +1991,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="576">
@@ -4686,7 +4697,7 @@
   <dimension ref="A1:BT12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5238,7 +5249,7 @@
         <f>HYPERLINK("https://upload.wikimedia.org/wikipedia/commons/thumb/d/da/4Messer_fcm.png/150px-4Messer_fcm.png")</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/d/da/4Messer_fcm.png/150px-4Messer_fcm.png</v>
       </c>
-      <c r="L3" t="str">
+      <c r="L3" s="3" t="str">
         <f>HYPERLINK("https://www.ingenieur.de/wp-content/uploads/2017/11/2016/17082_E-Traktor-von-John-Deere.jpg")</f>
         <v>https://www.ingenieur.de/wp-content/uploads/2017/11/2016/17082_E-Traktor-von-John-Deere.jpg</v>
       </c>
@@ -6795,10 +6806,118 @@
       <c r="A11" t="s">
         <v>612</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>613</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6814,7 +6933,7 @@
   <dimension ref="A1:BT12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8922,10 +9041,118 @@
       <c r="A11" t="s">
         <v>612</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>613</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8941,7 +9168,7 @@
   <dimension ref="A1:BT12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9476,7 +9703,7 @@
         <f>HYPERLINK("https://upload.wikimedia.org/wikipedia/commons/9/9b/Wild_Pig_KSC02pd0873.jpg")</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/9/9b/Wild_Pig_KSC02pd0873.jpg</v>
       </c>
-      <c r="H3" t="str">
+      <c r="H3" s="3" t="str">
         <f>HYPERLINK("https://upload.wikimedia.org/wikipedia/commons/thumb/4/4d/Racemic_methamphetamine.svg/1920px-Racemic_methamphetamine.svg.png")</f>
         <v>https://upload.wikimedia.org/wikipedia/commons/thumb/4/4d/Racemic_methamphetamine.svg/1920px-Racemic_methamphetamine.svg.png</v>
       </c>
@@ -11049,10 +11276,118 @@
       <c r="A11" t="s">
         <v>612</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>613</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -11068,7 +11403,7 @@
   <dimension ref="A1:BT12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13177,10 +13512,118 @@
       <c r="A11" t="s">
         <v>612</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>613</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -13196,7 +13639,7 @@
   <dimension ref="A1:BT12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15305,10 +15748,118 @@
       <c r="A11" t="s">
         <v>612</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>613</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -15324,7 +15875,7 @@
   <dimension ref="A1:BT12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17432,10 +17983,118 @@
       <c r="A11" t="s">
         <v>612</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>613</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -17451,7 +18110,7 @@
   <dimension ref="A1:BT12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19559,10 +20218,118 @@
       <c r="A11" t="s">
         <v>612</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>613</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -19577,8 +20344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41344A75-69A0-494A-87C9-2B407DF4026F}">
   <dimension ref="A1:BT12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21686,10 +22453,118 @@
       <c r="A11" t="s">
         <v>612</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>613</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -21704,8 +22579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A549D88-9782-4382-B82A-DD67F5D5D994}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21750,35 +22625,35 @@
       </c>
       <c r="B4">
         <f>SUM('VGG 16'!B11:BT11)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <f>SUM('VGG 19'!B11:BT11)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <f>SUM('MobileNet V2'!B11:BT11)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <f>SUM('ResNet 50'!B11:BT11)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <f>SUM('DenseNet 201'!B11:BT11)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G4">
         <f>SUM('Inception V3'!B11:BT11)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H4">
         <f>SUM(Xception!B11:BT11)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I4">
         <f>SUM(InceptionResnet!B11:BT11)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -21787,35 +22662,35 @@
       </c>
       <c r="B5">
         <f>SUM('VGG 16'!B12:BT12)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <f>SUM('VGG 19'!B12:BT12)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <f>SUM('MobileNet V2'!B12:BT12)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <f>SUM('ResNet 50'!B12:BT12)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <f>SUM('DenseNet 201'!B12:BT12)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G5">
         <f>SUM('Inception V3'!B12:BT12)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H5">
         <f>SUM(Xception!B12:BT12)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I5">
         <f>SUM(InceptionResnet!B12:BT12)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>